<commit_message>
Final analysis pt 1000
- Finalised evap analysis
- Script to calculate and plot co2 emi and land use
</commit_message>
<xml_diff>
--- a/HydroFPV_plants/EvapAnalysis/EvapReductions_ref.xlsx
+++ b/HydroFPV_plants/EvapAnalysis/EvapReductions_ref.xlsx
@@ -14,9 +14,13 @@
     <sheet name="Reductions mcm" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Reductions mm" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Extra HP generation PJ" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Max extra HP generation PJ" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Extra HP generation %" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Max extra HP generation %" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Extra HP generation %" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Max values" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Max values EG" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Max values ET" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Max values SD" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Max values overv" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Tot values overv" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,238 +465,1160 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Installed FPV capacity [GW]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>FPV coverage area [%]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Reservoir evaporation [mcm/y]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [mcm/y]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Evaporation reduction [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [PJ/y]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [% of HP]</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Amarti-Neshe</t>
+          <t>Aswan1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.28</v>
+      </c>
+      <c r="C2" t="n">
+        <v>33.98058252427185</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9.0392299323409</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.914561405647103</v>
+      </c>
+      <c r="F2" t="n">
+        <v>54.36924873504544</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.02444163492762758</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.2913672713876879</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Aswan1</t>
+          <t>Aswan2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2913672713876879</v>
+        <v>0.27</v>
+      </c>
+      <c r="C3" t="n">
+        <v>32.76699029126214</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9.0392299323409</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.769213184332382</v>
+      </c>
+      <c r="F3" t="n">
+        <v>52.76127745427639</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.02301729019228999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.2845505030571144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Aswan2</t>
+          <t>HighAswanDam</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2845505030571144</v>
+        <v>2.100000000000028</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3230769230769274</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7130.460504880564</v>
+      </c>
+      <c r="E4" t="n">
+        <v>43.31831778134737</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6075108017455173</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.002407230860169421</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.005308596499726372</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Baro</t>
+          <t>tot</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01668182242325251</v>
+        <v>2.650000000000028</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.008133225299548309</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7148.538964745246</v>
+      </c>
+      <c r="E5" t="n">
+        <v>53.00209237132686</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.7414395113843477</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.04986615598008699</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1613178030363437</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Installed FPV capacity [GW]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>FPV coverage area [%]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Reservoir evaporation [mcm/y]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [mcm/y]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Evaporation reduction [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [PJ/y]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [% of HP]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Finchaa</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="C2" t="n">
+        <v>62.74509803921568</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9577781845919145</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8054522427359775</v>
+      </c>
+      <c r="F2" t="n">
+        <v>84.09590609741865</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0026517791764049</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.1500299392591174</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>LakeTana-Beles</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.4600000000000227</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1277777777777841</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1690.196796338673</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.064572173332208</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.2404792259775276</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3.826618012809465e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.001291859833499701</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Tekeze1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.325581395348837</v>
+      </c>
+      <c r="D4" t="n">
+        <v>60.56538520213577</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.625112630914142</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.334344811236453</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0004454450180301331</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.006249228648009724</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Amarti-Neshe</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10.61067988812611</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Dagash</t>
+          <t>Renaissance</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5553633613957271</v>
+        <v>6.400000000000024</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.415154749199586</v>
+      </c>
+      <c r="D6" t="n">
+        <v>879.8413323162979</v>
+      </c>
+      <c r="E6" t="n">
+        <v>55.73055230702768</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6.334159383068499</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.01381990446020911</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.06812331519431067</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Dal</t>
+          <t>Baro</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5479799900611368</v>
+        <v>0.645</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.908390125002099</v>
+      </c>
+      <c r="D7" t="n">
+        <v>77.48124325498756</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.604190209698729</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7.232963713883075</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.001586908403479165</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.01668182242325251</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Finchaa</t>
+          <t>Tekeze2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1500299392591174</v>
+        <v>0.38</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.943731911520321</v>
+      </c>
+      <c r="D8" t="n">
+        <v>45.23879052594407</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.301169781616321</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7.297210520522487</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0009430776293140112</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.01320652050572765</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>HighAswanDam</t>
+          <t>tot</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.005308596499726372</v>
+        <v>8.313000000000049</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.02823217756173276</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2764.892005710756</v>
+      </c>
+      <c r="E9" t="n">
+        <v>72.13104934532507</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2.608819772936583</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.01948538086756542</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.04013107140259403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Installed FPV capacity [GW]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>FPV coverage area [%]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Reservoir evaporation [mcm/y]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [mcm/y]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Evaporation reduction [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [PJ/y]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [% of HP]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Sennar</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.710526315789473</v>
+      </c>
+      <c r="D2" t="n">
+        <v>51.91592593523102</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.659626985942905</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.196758905953855</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.001511002980671087</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.3879340130092649</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>KashmElGirba</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.07999999999999999</v>
+      </c>
+      <c r="D3" t="n">
+        <v>426.940180388413</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6429404287121326</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1505926259100775</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.757524571715746e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.01278407311875636</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Roseires</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.384548049496758</v>
+      </c>
+      <c r="D4" t="n">
+        <v>795.8164962440018</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.7529920715873</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.722904350279188</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.001184457720485239</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.02928564026419185</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>JebelAulia</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.01554828150572831</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4173.767203477125</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.221933908021235</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.02927652282578804</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.018854481387687e-05</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.002794444545769849</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Merowe</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.240000000000034</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.605042016806794</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1625.788206919077</v>
+      </c>
+      <c r="E6" t="n">
+        <v>78.8369119720152</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.849150192903282</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1088780138247659</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.4017950240600414</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>UpperAtbara</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>341.5521443107304</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20.29101434587296</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5.940824756589145</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.03433171107063304</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.308672374423764</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Kajbar</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.272727272727272</v>
+      </c>
+      <c r="D8" t="n">
+        <v>375.7073587418034</v>
+      </c>
+      <c r="E8" t="n">
+        <v>22.81996523908077</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.07386698932434</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.03947527871342674</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.4615048484080007</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Shereik</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4200000000000013</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.935482686702886</v>
+      </c>
+      <c r="D9" t="n">
+        <v>364.5090374687685</v>
+      </c>
+      <c r="E9" t="n">
+        <v>26.54433672887577</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7.282216351398452</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.05505292582400474</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.557644805964146</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>JebelAulia</t>
+          <t>Dagash</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.002794444545769849</v>
+        <v>0.312</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.962740698618387</v>
+      </c>
+      <c r="D10" t="n">
+        <v>268.9155741684072</v>
+      </c>
+      <c r="E10" t="n">
+        <v>19.71623766502704</v>
+      </c>
+      <c r="F10" t="n">
+        <v>7.331757458078584</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.04116964134362664</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.5553633613957271</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Kajbar</t>
+          <t>Dal</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4615048484080007</v>
+        <v>0.648</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.908157617400247</v>
+      </c>
+      <c r="D11" t="n">
+        <v>566.3174599917538</v>
+      </c>
+      <c r="E11" t="n">
+        <v>40.95914235011031</v>
+      </c>
+      <c r="F11" t="n">
+        <v>7.232540976346856</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.08436973916976293</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5479799900611368</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>KashmElGirba</t>
+          <t>Mograt</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01278407311875636</v>
+        <v>0.312</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.962740698618387</v>
+      </c>
+      <c r="D12" t="n">
+        <v>268.9155741684072</v>
+      </c>
+      <c r="E12" t="n">
+        <v>19.71623766502704</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7.331757458078584</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.04116964134362664</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.072992294394606</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>LakeTana-Beles</t>
+          <t>Sabaloka</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.001291859833499701</v>
+        <v>0.205</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.933134957099713</v>
+      </c>
+      <c r="D13" t="n">
+        <v>362.20021435414</v>
+      </c>
+      <c r="E13" t="n">
+        <v>13.07258100692888</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3.609214044845155</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0134375140003368</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.275878993190786</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Merowe</t>
+          <t>tot</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4017950240600414</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Mograt</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1.072992294394606</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Renaissance</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.06812331519431067</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Roseires</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.02928564026419185</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Sabaloka</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.275878993190786</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Sennar</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.3879340130092649</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Shereik</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0.557644805964146</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Tekeze1</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0.006249228648009724</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Tekeze2</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.01320652050572765</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>UpperAtbara</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1.308672374423764</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>tot</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.2458047161502279</v>
+        <v>4.142000000000035</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.02940466022429287</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9622.345376167857</v>
+      </c>
+      <c r="E14" t="n">
+        <v>251.2339203672016</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.610942660501931</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.4206176897818709</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.8120220734493289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENB</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>EG</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ET</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Installed FPV capacity [GW]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>15.10500000000011</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.650000000000028</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8.313000000000049</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.142000000000035</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>FPV coverage area [%]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.01984530316185869</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.008133225299548309</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.02823217756173276</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.02940466022429287</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Reservoir evaporation [mcm/y]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>19535.77634662386</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7148.538964745246</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2764.892005710756</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9622.345376167857</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [mcm/y]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>376.3670620838534</v>
+      </c>
+      <c r="C5" t="n">
+        <v>53.00209237132686</v>
+      </c>
+      <c r="D5" t="n">
+        <v>72.13104934532507</v>
+      </c>
+      <c r="E5" t="n">
+        <v>251.2339203672016</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Evaporation reduction [%]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.926552881267483</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7414395113843477</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.608819772936583</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.610942660501931</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [PJ/y]</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4899692266295232</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.04986615598008699</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.01948538086756542</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.4206176897818709</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [% of HP]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.3732675122058701</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1613178030363437</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.04013107140259403</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8120220734493289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENB</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>EG</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ET</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Reservoir evaporation [mcm]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>799705.0038191883</v>
+      </c>
+      <c r="C2" t="n">
+        <v>307387.1754840456</v>
+      </c>
+      <c r="D2" t="n">
+        <v>118632.4650616009</v>
+      </c>
+      <c r="E2" t="n">
+        <v>373685.3632735417</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [mcm]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11449.46430985102</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1855.143822557379</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1421.852020408626</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8172.468466885013</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [%]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.431710975318559</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.6035202410888045</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.198535341628716</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.186991857345689</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [PJ]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>15.7535948568749</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.742568262187653</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.297234309312523</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.71379228537472</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [% of HP]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1536649772013688</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.06554925442055143</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.008218098568986181</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.344855877289768</v>
       </c>
     </row>
   </sheetData>
@@ -20842,260 +21768,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Amarti-Neshe</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Aswan1</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.8554572224669656</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Aswan2</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.8056051567301499</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Baro</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.01428217563131248</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Dagash</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1.416406447386402</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Dal</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2.79077872342501</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Finchaa</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.0079553375292147</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>HighAswanDam</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.08150588299053803</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>JebelAulia</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.0003260334340440597</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Kajbar</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1.4422675815397</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>KashmElGirba</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.0002206019657372597</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>LakeTana-Beles</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.001157742337681779</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Merowe</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>3.682631971815895</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Mograt</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1.067356782802781</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Renaissance</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.2520808551181488</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Roseires</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.008295025151366799</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Sabaloka</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.4356615141654023</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Sennar</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.006044011922684348</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Shereik</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1.842537363357799</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Tekeze1</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0.005790785234391731</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Tekeze2</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.01596741346177342</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>UpperAtbara</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1.021266228407901</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>tot</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>15.7535948568749</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24269,4 +24941,702 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Installed FPV capacity [GW]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>FPV coverage area [%]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Reservoir evaporation [mcm/y]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Water savings [mcm/y]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Evaporation reduction [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [PJ/y]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Extra hp generation [% of HP]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Aswan1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="C2" t="n">
+        <v>33.98058252427185</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9.0392299323409</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.914561405647103</v>
+      </c>
+      <c r="F2" t="n">
+        <v>54.36924873504544</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.02444163492762758</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.2913672713876879</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Aswan2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="C3" t="n">
+        <v>32.76699029126214</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9.0392299323409</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.769213184332382</v>
+      </c>
+      <c r="F3" t="n">
+        <v>52.76127745427639</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.02301729019228999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.2845505030571144</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Baro</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.908390125002099</v>
+      </c>
+      <c r="D4" t="n">
+        <v>77.48124325498756</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.604190209698729</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7.232963713883075</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.001586908403479165</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.01668182242325251</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Dagash</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.962740698618387</v>
+      </c>
+      <c r="D5" t="n">
+        <v>268.9155741684072</v>
+      </c>
+      <c r="E5" t="n">
+        <v>19.71623766502704</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.331757458078584</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.04116964134362664</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5553633613957271</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Dal</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.648</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.908157617400247</v>
+      </c>
+      <c r="D6" t="n">
+        <v>566.3174599917538</v>
+      </c>
+      <c r="E6" t="n">
+        <v>40.95914235011031</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7.232540976346856</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.08436973916976293</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5479799900611368</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Finchaa</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="C7" t="n">
+        <v>62.74509803921568</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9577781845919145</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8054522427359775</v>
+      </c>
+      <c r="F7" t="n">
+        <v>84.09590609741865</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0026517791764049</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.1500299392591174</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>HighAswanDam</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.100000000000028</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.3230769230769274</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7130.460504880564</v>
+      </c>
+      <c r="E8" t="n">
+        <v>43.31831778134737</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6075108017455173</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.002407230860169421</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.005308596499726372</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>JebelAulia</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.01554828150572831</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4173.767203477125</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.221933908021235</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.02927652282578804</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.018854481387687e-05</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.002794444545769849</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Kajbar</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.272727272727272</v>
+      </c>
+      <c r="D10" t="n">
+        <v>375.7073587418034</v>
+      </c>
+      <c r="E10" t="n">
+        <v>22.81996523908077</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6.07386698932434</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.03947527871342674</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.4615048484080007</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>KashmElGirba</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.07999999999999999</v>
+      </c>
+      <c r="D11" t="n">
+        <v>426.940180388413</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6429404287121326</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1505926259100775</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.757524571715746e-05</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.01278407311875636</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>LakeTana-Beles</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.4600000000000227</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.1277777777777841</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1690.196796338673</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4.064572173332208</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.2404792259775276</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3.826618012809465e-05</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.001291859833499701</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Merowe</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.240000000000034</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.605042016806794</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1625.788206919077</v>
+      </c>
+      <c r="E13" t="n">
+        <v>78.8369119720152</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.849150192903282</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1088780138247659</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.4017950240600414</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Mograt</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.962740698618387</v>
+      </c>
+      <c r="D14" t="n">
+        <v>268.9155741684072</v>
+      </c>
+      <c r="E14" t="n">
+        <v>19.71623766502704</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.331757458078584</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.04116964134362664</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.072992294394606</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Renaissance</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>6.400000000000024</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3.415154749199586</v>
+      </c>
+      <c r="D15" t="n">
+        <v>879.8413323162979</v>
+      </c>
+      <c r="E15" t="n">
+        <v>55.73055230702768</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6.334159383068499</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.01381990446020911</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.06812331519431067</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Roseires</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.384548049496758</v>
+      </c>
+      <c r="D16" t="n">
+        <v>795.8164962440018</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5.7529920715873</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.722904350279188</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.001184457720485239</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.02928564026419185</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Sabaloka</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.933134957099713</v>
+      </c>
+      <c r="D17" t="n">
+        <v>362.20021435414</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.07258100692888</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3.609214044845155</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0134375140003368</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.275878993190786</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Sennar</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.710526315789473</v>
+      </c>
+      <c r="D18" t="n">
+        <v>51.91592593523102</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.659626985942905</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3.196758905953855</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.001511002980671087</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.3879340130092649</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Shereik</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.4200000000000013</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.935482686702886</v>
+      </c>
+      <c r="D19" t="n">
+        <v>364.5090374687685</v>
+      </c>
+      <c r="E19" t="n">
+        <v>26.54433672887577</v>
+      </c>
+      <c r="F19" t="n">
+        <v>7.282216351398452</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.05505292582400474</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.557644805964146</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Tekeze1</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2.325581395348837</v>
+      </c>
+      <c r="D20" t="n">
+        <v>60.56538520213577</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.625112630914142</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.334344811236453</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0004454450180301331</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.006249228648009724</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Tekeze2</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3.943731911520321</v>
+      </c>
+      <c r="D21" t="n">
+        <v>45.23879052594407</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.301169781616321</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7.297210520522487</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0009430776293140112</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.01320652050572765</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>UpperAtbara</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D22" t="n">
+        <v>341.5521443107304</v>
+      </c>
+      <c r="E22" t="n">
+        <v>20.29101434587296</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5.940824756589145</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.03433171107063304</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.308672374423764</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Amarti-Neshe</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>10.61067988812611</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>tot</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>15.10500000000011</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.01984530316185869</v>
+      </c>
+      <c r="D24" t="n">
+        <v>19535.77634662386</v>
+      </c>
+      <c r="E24" t="n">
+        <v>376.3670620838534</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.926552881267483</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.4899692266295232</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.3732675122058701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>